<commit_message>
created pdf_manager for lambdas
</commit_message>
<xml_diff>
--- a/pdf-manager/Devin's Form.xlsx
+++ b/pdf-manager/Devin's Form.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>First Name</t>
   </si>
@@ -29,21 +29,6 @@
   </si>
   <si>
     <t>Likes Dogs</t>
-  </si>
-  <si>
-    <t>firsttest</t>
-  </si>
-  <si>
-    <t>lasttest</t>
-  </si>
-  <si>
-    <t>123 sesame st</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -375,7 +360,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,7 +368,7 @@
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -405,23 +390,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>